<commit_message>
removed NULL values for connectors for a uniform doc pattern
</commit_message>
<xml_diff>
--- a/data/JAUNT_ParaServiceAreaRules.xlsx
+++ b/data/JAUNT_ParaServiceAreaRules.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Administration\Mobility Manager\Technology\Civic Innovation Day\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanday/future/cid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5444F846-661A-4586-B826-DFD8CEBEA6E8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="135">
   <si>
     <t>ParaServiceId</t>
   </si>
@@ -435,7 +440,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,27 +505,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R45" totalsRowShown="0">
-  <autoFilter ref="A1:R45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:R45" totalsRowShown="0">
+  <autoFilter ref="A1:R45"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ParaServiceId"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParaServiceAbbr"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ParaServiceDescription"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="serviceAreaRuleId"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ParaServiceAreaRuleDescription"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="EffectiveFromDate"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EffectiveToDate"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="WeekTemplate"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="TrapezeFromPolyId"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="GISFromPolyId"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="FromPolyName"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="TrapezeToPolyId"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="GISToPolyId"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="ToPolyName"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="FromTime" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="ToTime" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ReverseFromTime" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ReverseToTime" dataDxfId="0"/>
+    <tableColumn id="1" name="ParaServiceId"/>
+    <tableColumn id="2" name="ParaServiceAbbr"/>
+    <tableColumn id="3" name="ParaServiceDescription"/>
+    <tableColumn id="4" name="serviceAreaRuleId"/>
+    <tableColumn id="5" name="ParaServiceAreaRuleDescription"/>
+    <tableColumn id="6" name="EffectiveFromDate"/>
+    <tableColumn id="7" name="EffectiveToDate"/>
+    <tableColumn id="8" name="WeekTemplate"/>
+    <tableColumn id="9" name="TrapezeFromPolyId"/>
+    <tableColumn id="10" name="GISFromPolyId"/>
+    <tableColumn id="11" name="FromPolyName"/>
+    <tableColumn id="12" name="TrapezeToPolyId"/>
+    <tableColumn id="13" name="GISToPolyId"/>
+    <tableColumn id="14" name="ToPolyName"/>
+    <tableColumn id="15" name="FromTime" dataDxfId="3"/>
+    <tableColumn id="16" name="ToTime" dataDxfId="2"/>
+    <tableColumn id="17" name="ReverseFromTime" dataDxfId="1"/>
+    <tableColumn id="18" name="ReverseToTime" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -788,36 +793,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="14" max="14" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -929,7 +934,7 @@
         <v>0.76041666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -982,7 +987,7 @@
         <v>0.74652777777777779</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1038,7 +1043,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1094,7 +1099,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1150,7 +1155,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1206,7 +1211,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1262,7 +1267,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1318,7 +1323,7 @@
         <v>0.76388888888888884</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1374,7 +1379,7 @@
         <v>0.69791666666666663</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1430,7 +1435,7 @@
         <v>0.69791666666666663</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>13</v>
       </c>
@@ -1486,7 +1491,7 @@
         <v>0.77083333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>14</v>
       </c>
@@ -1542,7 +1547,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>15</v>
       </c>
@@ -1598,7 +1603,7 @@
         <v>0.73958333333333337</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
@@ -1654,7 +1659,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1710,7 +1715,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1766,7 +1771,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1822,7 +1827,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1878,7 +1883,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1934,7 +1939,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1990,7 +1995,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2046,7 +2051,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2102,7 +2107,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2158,7 +2163,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2214,7 +2219,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2270,7 +2275,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2326,7 +2331,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>24</v>
       </c>
@@ -2382,7 +2387,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2438,7 +2443,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>25</v>
       </c>
@@ -2487,14 +2492,14 @@
       <c r="P30" s="1">
         <v>0.39583333333333331</v>
       </c>
-      <c r="Q30" t="s">
-        <v>17</v>
-      </c>
-      <c r="R30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q30" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>27</v>
       </c>
@@ -2550,7 +2555,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>27</v>
       </c>
@@ -2606,7 +2611,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>27</v>
       </c>
@@ -2662,7 +2667,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>28</v>
       </c>
@@ -2718,7 +2723,7 @@
         <v>0.97916666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>28</v>
       </c>
@@ -2774,7 +2779,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>29</v>
       </c>
@@ -2830,7 +2835,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>30</v>
       </c>
@@ -2886,7 +2891,7 @@
         <v>0.75694444444444453</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>31</v>
       </c>
@@ -2942,7 +2947,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>31</v>
       </c>
@@ -2991,14 +2996,14 @@
       <c r="P39" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="Q39" t="s">
-        <v>17</v>
-      </c>
-      <c r="R39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q39" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="R39" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>32</v>
       </c>
@@ -3054,7 +3059,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>33</v>
       </c>
@@ -3110,7 +3115,7 @@
         <v>0.97916666666666663</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>33</v>
       </c>
@@ -3166,7 +3171,7 @@
         <v>0.97916666666666663</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>33</v>
       </c>
@@ -3222,7 +3227,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>33</v>
       </c>
@@ -3278,7 +3283,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>34</v>
       </c>

</xml_diff>